<commit_message>
Update Mode of operation variables
</commit_message>
<xml_diff>
--- a/t1_confection/Miscellaneous/A-Xtra_Emissions.xlsx
+++ b/t1_confection/Miscellaneous/A-Xtra_Emissions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\relac_tx\t1_confection\Miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06BCCB1-67CA-419B-AF8C-F01DDF49FF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD56D051-05D2-4611-870E-32FD0708D693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GHGs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>External Cost</t>
   </si>
@@ -202,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,10 +211,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -505,41 +503,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="3"/>
     </row>
   </sheetData>
@@ -553,20 +551,23 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -574,12 +575,15 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -791,15 +795,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="48eed89a-7418-4977-ae3a-838f0fac8ec5">
@@ -808,6 +803,15 @@
     <TaxCatchAll xmlns="416d42ac-85ec-40c4-8054-6c816fd4b6a7" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -830,14 +834,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F79AB8-49D9-484F-991A-27FAE0E62C64}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFFB2CC7-4028-40CF-B585-77900DA351B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -847,4 +843,12 @@
     <ds:schemaRef ds:uri="416d42ac-85ec-40c4-8054-6c816fd4b6a7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F79AB8-49D9-484F-991A-27FAE0E62C64}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add new modules to include some variables as EmissionPenalty DaySplit. Also, check the manage of a few variables as timelsices to SpecifiedAnnualDemand
</commit_message>
<xml_diff>
--- a/t1_confection/Miscellaneous/A-Xtra_Emissions.xlsx
+++ b/t1_confection/Miscellaneous/A-Xtra_Emissions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\relac_tx\t1_confection\Miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD56D051-05D2-4611-870E-32FD0708D693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC7B706-98B8-4D47-811D-D25E03390765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22104" yWindow="936" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GHGs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>External Cost</t>
   </si>
@@ -507,17 +507,17 @@
       <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="5"/>
@@ -551,39 +551,44 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -795,6 +800,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="48eed89a-7418-4977-ae3a-838f0fac8ec5">
@@ -803,15 +817,6 @@
     <TaxCatchAll xmlns="416d42ac-85ec-40c4-8054-6c816fd4b6a7" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -834,6 +839,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F79AB8-49D9-484F-991A-27FAE0E62C64}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFFB2CC7-4028-40CF-B585-77900DA351B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -843,12 +856,4 @@
     <ds:schemaRef ds:uri="416d42ac-85ec-40c4-8054-6c816fd4b6a7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F79AB8-49D9-484F-991A-27FAE0E62C64}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>